<commit_message>
Fixed items still displaying as JSON objects in Excel
</commit_message>
<xml_diff>
--- a/backend/my_selected_milestones.xlsx
+++ b/backend/my_selected_milestones.xlsx
@@ -16,16 +16,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>{'milestone': 'Milestone 1'}</t>
-  </si>
-  <si>
-    <t>{'milestone': 'Milestone 3'}</t>
-  </si>
-  <si>
-    <t>{'date': '2022-01-15'}</t>
-  </si>
-  <si>
-    <t>{}</t>
+    <t>Milestone 1</t>
+  </si>
+  <si>
+    <t>Milestone 3</t>
+  </si>
+  <si>
+    <t>Milestone 5</t>
+  </si>
+  <si>
+    <t>2022-01-15</t>
   </si>
   <si>
     <t>Selected milestone(s)</t>
@@ -79,8 +79,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B3" totalsRowShown="0">
-  <autoFilter ref="A1:B3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B4" totalsRowShown="0">
+  <autoFilter ref="A1:B4"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Selected milestone(s)"/>
     <tableColumn id="2" name="Selected completion date"/>
@@ -374,7 +374,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -396,15 +396,17 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>